<commit_message>
beginning of sims for cardmatch
note: profmatch has yet to be implemented
</commit_message>
<xml_diff>
--- a/Data Collection.xlsx
+++ b/Data Collection.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\GitHub\Stat-293\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE0A3E5-32C5-4043-B46D-56AA0D1E52E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6787676-8D36-47F5-8295-236ED72F20BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="290" windowWidth="15840" windowHeight="9580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="290" windowWidth="15840" windowHeight="9580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BMatch" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="CardMatch" sheetId="4" r:id="rId2"/>
     <sheet name="Variable Selection Methods" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="17">
   <si>
     <t>Sample:</t>
   </si>
@@ -400,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="A1:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -988,13 +988,481 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92C43F1-8811-4254-97AD-EDF825DF7EAB}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D95F620-68B2-4399-B918-51914767375A}">
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" customWidth="1"/>
+    <col min="10" max="10" width="23.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>4.2910400000000001E-2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>2.3436740000000001E-2</v>
+      </c>
+      <c r="J3">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>1.7760739999999999</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>0.78886109999999998</v>
+      </c>
+      <c r="J4">
+        <v>395.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2000</v>
+      </c>
+      <c r="B5">
+        <v>0.2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>12.860099999999999</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>8.4210499999999993</v>
+      </c>
+      <c r="J5">
+        <v>777.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3000</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>20.335999999999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>10.36347</v>
+      </c>
+      <c r="J6">
+        <v>1183.5999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5000</v>
+      </c>
+      <c r="B7">
+        <v>0.2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8">
+        <v>0.2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9">
+        <v>0.2</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>3000</v>
+      </c>
+      <c r="B10">
+        <v>0.2</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <v>0.2</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>0.2</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>3000</v>
+      </c>
+      <c r="B13">
+        <v>0.2</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>0.2</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1000</v>
+      </c>
+      <c r="B15">
+        <v>0.2</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>3000</v>
+      </c>
+      <c r="B16">
+        <v>0.2</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1000</v>
+      </c>
+      <c r="B17">
+        <v>0.2</v>
+      </c>
+      <c r="C17">
+        <v>200</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>3000</v>
+      </c>
+      <c r="B18">
+        <v>0.2</v>
+      </c>
+      <c r="C18">
+        <v>600</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>